<commit_message>
Adding file for storing timber properties + modifying building configs files
</commit_message>
<xml_diff>
--- a/Building_Configurations.xlsx
+++ b/Building_Configurations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SATNOORK\Documents\GitHub\CLT-LCA-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E33F91-07E5-4757-8967-CEAEF65B70BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E341AE03-C0DA-4AD1-A072-A8E85902B9F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Index" sheetId="1" r:id="rId1"/>
+    <sheet name="Lever_CLT" sheetId="2" r:id="rId2"/>
+    <sheet name="Lever_Concrete" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="73">
   <si>
     <t>Index</t>
   </si>
@@ -232,9 +233,6 @@
     <t>Concrete Masonry Unit</t>
   </si>
   <si>
-    <t>m4</t>
-  </si>
-  <si>
     <t>Silicone Sealant</t>
   </si>
   <si>
@@ -245,6 +243,18 @@
   </si>
   <si>
     <t>Floor Area_m</t>
+  </si>
+  <si>
+    <t>Quantity_LCA</t>
+  </si>
+  <si>
+    <t>Normalized_Quantity_LCA_1</t>
+  </si>
+  <si>
+    <t>Lever Concrete</t>
+  </si>
+  <si>
+    <t>sqm</t>
   </si>
 </sst>
 </file>
@@ -302,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -331,12 +341,147 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -666,7 +811,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,10 +843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AB2A63-0E4D-4D7F-9DC1-611AEDADC1C9}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +860,7 @@
     <col min="7" max="16384" width="15.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -729,8 +874,9 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -744,8 +890,9 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -759,8 +906,9 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -774,10 +922,11 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5">
         <f>B6/0.0929</f>
@@ -791,9 +940,9 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2">
         <v>8360</v>
@@ -805,8 +954,9 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -820,8 +970,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -830,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -859,22 +1010,22 @@
         <v>22</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="K10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -894,22 +1045,27 @@
       <c r="G11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="7">
+        <f>E11</f>
+        <v>11449</v>
+      </c>
+      <c r="K11" s="3">
         <f>F11</f>
         <v>11449</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="3">
-        <f>J11</f>
+      <c r="L11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3">
+        <f>K11</f>
         <v>11449</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -932,22 +1088,27 @@
       <c r="I12" s="3">
         <v>450</v>
       </c>
-      <c r="J12" s="3">
-        <f t="shared" ref="J12:J49" si="0">F12</f>
+      <c r="J12" s="10">
+        <f t="shared" ref="J12:J50" si="0">E12</f>
         <v>0.95</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="3">
+        <f>F12</f>
+        <v>0.95</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="3">
-        <f>I12*J12</f>
+      <c r="M12" s="3">
+        <f>I12*K12</f>
         <v>427.5</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -973,22 +1134,27 @@
       <c r="I13" s="3">
         <v>70</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="10">
+        <f>E13*H13*I13</f>
+        <v>506.73</v>
+      </c>
+      <c r="K13" s="3">
         <f>F13*H13*I13</f>
         <v>506.73</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="3">
-        <f>J13</f>
+      <c r="L13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="3">
+        <f>K13</f>
         <v>506.73</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -1011,22 +1177,27 @@
       <c r="I14" s="3">
         <v>1198.26</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="7">
+        <f>E14*I14/1000</f>
+        <v>3709.8129599999997</v>
+      </c>
+      <c r="K14" s="3">
         <f>F14/1000*I14</f>
         <v>3709.8129600000002</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="3">
-        <f t="shared" ref="L14:L19" si="1">J14</f>
+      <c r="L14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" ref="M14:M19" si="1">K14</f>
         <v>3709.8129600000002</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1052,22 +1223,27 @@
       <c r="I15" s="3">
         <v>30</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="10">
+        <f>E15*H15*I15</f>
+        <v>109.72799999999999</v>
+      </c>
+      <c r="K15" s="3">
         <f>F15*H15*I15</f>
         <v>109.72799999999999</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="3">
+      <c r="L15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="3">
         <f t="shared" si="1"/>
         <v>109.72799999999999</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1087,22 +1263,27 @@
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="7">
         <f t="shared" si="0"/>
         <v>5693</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="3">
+      <c r="K16" s="3">
+        <f>F16</f>
+        <v>5693</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="3">
         <f t="shared" si="1"/>
         <v>5693</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -1129,22 +1310,27 @@
       <c r="I17" s="1">
         <v>675</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="10">
+        <f>E17*H17*I17</f>
+        <v>159737.82187499999</v>
+      </c>
+      <c r="K17" s="3">
         <f>F17*H17*I17</f>
         <v>159737.82187499999</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="3">
+      <c r="L17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="3">
         <f t="shared" si="1"/>
         <v>159737.82187499999</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -1171,22 +1357,27 @@
       <c r="I18" s="1">
         <v>675</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="10">
+        <f>E18*H18*I18</f>
+        <v>35610.165000000001</v>
+      </c>
+      <c r="K18" s="3">
         <f>F18*H18*I18</f>
         <v>35610.165000000001</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="L18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="3">
         <f t="shared" si="1"/>
         <v>35610.165000000001</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -1209,22 +1400,27 @@
       <c r="I19" s="3">
         <v>1200</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="7">
+        <f>E19*I19/1000</f>
+        <v>140.4</v>
+      </c>
+      <c r="K19" s="3">
         <f>F19/1000*I19</f>
         <v>140.4</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="3">
+      <c r="L19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" s="3">
         <f t="shared" si="1"/>
         <v>140.4</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1247,22 +1443,27 @@
       <c r="I20" s="3">
         <v>450</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="7">
         <f t="shared" si="0"/>
         <v>1279</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="3">
+        <f>F20</f>
+        <v>1279</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="3">
-        <f>I20*J20</f>
+      <c r="M20" s="3">
+        <f>I20*K20</f>
         <v>575550</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1282,22 +1483,27 @@
       <c r="G21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="7">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21" s="3">
-        <f>J21</f>
+      <c r="K21" s="3">
+        <f>F21</f>
         <v>110</v>
       </c>
-      <c r="M21" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="3">
+        <f>K21</f>
+        <v>110</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>44</v>
       </c>
@@ -1317,22 +1523,27 @@
       <c r="G22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="K22" s="3">
         <f>F22</f>
         <v>400</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="3">
-        <f>J22</f>
+      <c r="L22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="3">
+        <f>K22</f>
         <v>400</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1355,22 +1566,27 @@
       <c r="I23" s="2">
         <v>2245</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="7">
         <f t="shared" si="0"/>
         <v>932</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="3">
+        <f>F23</f>
+        <v>932</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="3">
-        <f>I23*J23</f>
+      <c r="M23" s="3">
+        <f>I23*K23</f>
         <v>2092340</v>
       </c>
-      <c r="M23" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
@@ -1390,22 +1606,27 @@
       <c r="G24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="7">
         <f t="shared" si="0"/>
         <v>4737</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" s="3">
-        <f>J24</f>
+      <c r="K24" s="3">
+        <f>F24</f>
         <v>4737</v>
       </c>
-      <c r="M24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="3">
+        <f>K24</f>
+        <v>4737</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
@@ -1432,22 +1653,27 @@
       <c r="I25" s="3">
         <v>620</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="10">
+        <f>E25*H25*I25</f>
+        <v>3903.5354999999995</v>
+      </c>
+      <c r="K25" s="3">
         <f>F25*H25*I25</f>
         <v>3903.5354999999995</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" ref="L25:L30" si="2">J25</f>
+      <c r="L25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" ref="M25:M30" si="2">K25</f>
         <v>3903.5354999999995</v>
       </c>
-      <c r="M25" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
@@ -1473,22 +1699,27 @@
       <c r="I26" s="3">
         <v>30</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="10">
+        <f>E26*H26*I26</f>
+        <v>3099.0540000000001</v>
+      </c>
+      <c r="K26" s="3">
         <f>F26*H26*I26</f>
         <v>3099.0540000000001</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L26" s="3">
+      <c r="L26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="3">
         <f t="shared" si="2"/>
         <v>3099.0540000000001</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -1508,22 +1739,27 @@
       <c r="G27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="7">
         <f t="shared" si="0"/>
         <v>53177</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" s="3">
+      <c r="K27" s="3">
+        <f>F27</f>
+        <v>53177</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" s="3">
         <f t="shared" si="2"/>
         <v>53177</v>
       </c>
-      <c r="M27" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
@@ -1543,22 +1779,27 @@
       <c r="G28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="7">
         <f t="shared" si="0"/>
         <v>4193</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L28" s="3">
+      <c r="K28" s="3">
+        <f>F28</f>
+        <v>4193</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="3">
         <f t="shared" si="2"/>
         <v>4193</v>
       </c>
-      <c r="M28" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
@@ -1578,22 +1819,27 @@
       <c r="G29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="7">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L29" s="3">
+      <c r="K29" s="3">
+        <f>F29</f>
+        <v>110</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" s="3">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="M29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>44</v>
       </c>
@@ -1620,22 +1866,27 @@
       <c r="I30" s="3">
         <v>30</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="10">
+        <f>E30*H30*I30</f>
+        <v>16.047719999999998</v>
+      </c>
+      <c r="K30" s="3">
         <f>F30*H30*I30</f>
         <v>16.047719999999998</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L30" s="3">
+      <c r="L30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" s="3">
         <f t="shared" si="2"/>
         <v>16.047719999999998</v>
       </c>
-      <c r="M30" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1658,22 +1909,27 @@
       <c r="I31" s="2">
         <v>2245</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="7">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="3">
+        <f>F31</f>
+        <v>125</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L31" s="3">
-        <f>I31*J31</f>
+      <c r="M31" s="3">
+        <f>I31*K31</f>
         <v>280625</v>
       </c>
-      <c r="M31" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -1693,22 +1949,27 @@
       <c r="G32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="7">
         <f t="shared" si="0"/>
         <v>38590</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L32" s="3">
-        <f>J32</f>
+      <c r="K32" s="3">
+        <f>F32</f>
         <v>38590</v>
       </c>
-      <c r="M32" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32" s="3">
+        <f>K32</f>
+        <v>38590</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -1728,22 +1989,27 @@
       <c r="G33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="7">
         <f t="shared" si="0"/>
         <v>43527</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L33" s="3">
-        <f t="shared" ref="L33:L34" si="3">J33</f>
+      <c r="K33" s="3">
+        <f>F33</f>
         <v>43527</v>
       </c>
-      <c r="M33" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33" s="3">
+        <f t="shared" ref="M33:M34" si="3">K33</f>
+        <v>43527</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -1763,22 +2029,27 @@
       <c r="G34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="7">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L34" s="3">
+      <c r="K34" s="3">
+        <f>F34</f>
+        <v>60</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" s="3">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="M34" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -1801,22 +2072,27 @@
       <c r="I35" s="2">
         <v>2245</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="K35" s="3">
+        <f>F35</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L35" s="3">
-        <f>I35*J35</f>
+      <c r="M35" s="3">
+        <f>I35*K35</f>
         <v>0</v>
       </c>
-      <c r="M35" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -1839,22 +2115,27 @@
       <c r="I36" s="3">
         <v>450</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="7">
         <f t="shared" si="0"/>
         <v>557</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K36" s="3">
+        <f>F36</f>
+        <v>557</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L36" s="3">
-        <f>I36*J36</f>
+      <c r="M36" s="3">
+        <f>I36*K36</f>
         <v>250650</v>
       </c>
-      <c r="M36" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -1874,22 +2155,27 @@
       <c r="G37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L37" s="3">
-        <f>J37</f>
+      <c r="K37" s="3">
+        <f>F37</f>
         <v>0</v>
       </c>
-      <c r="M37" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" s="3">
+        <f>K37</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -1909,22 +2195,27 @@
       <c r="G38" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="7">
         <f t="shared" si="0"/>
         <v>830</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L38" s="3">
-        <f t="shared" ref="L38:L39" si="4">J38</f>
+      <c r="K38" s="3">
+        <f>F38</f>
         <v>830</v>
       </c>
-      <c r="M38" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" ref="M38:M39" si="4">K38</f>
+        <v>830</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>62</v>
       </c>
@@ -1944,22 +2235,27 @@
       <c r="G39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="7">
         <f t="shared" si="0"/>
         <v>31039</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="3">
+      <c r="K39" s="3">
+        <f>F39</f>
+        <v>31039</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39" s="3">
         <f t="shared" si="4"/>
         <v>31039</v>
       </c>
-      <c r="M39" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N39" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>62</v>
       </c>
@@ -1982,22 +2278,27 @@
       <c r="I40" s="3">
         <v>450</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="7">
         <f t="shared" si="0"/>
         <v>502</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="K40" s="3">
+        <f>F40</f>
+        <v>502</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L40" s="3">
-        <f>I40*J40</f>
+      <c r="M40" s="3">
+        <f>I40*K40</f>
         <v>225900</v>
       </c>
-      <c r="M40" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>62</v>
       </c>
@@ -2017,22 +2318,27 @@
       <c r="G41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="7">
         <f t="shared" si="0"/>
         <v>31947</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L41" s="3">
-        <f>J41</f>
+      <c r="K41" s="3">
+        <f>F41</f>
         <v>31947</v>
       </c>
-      <c r="M41" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M41" s="3">
+        <f>K41</f>
+        <v>31947</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>62</v>
       </c>
@@ -2055,22 +2361,27 @@
       <c r="I42" s="2">
         <v>2245</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="K42" s="3">
+        <f>F42</f>
+        <v>48</v>
+      </c>
+      <c r="L42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L42" s="3">
-        <f>I42*J42</f>
+      <c r="M42" s="3">
+        <f>I42*K42</f>
         <v>107760</v>
       </c>
-      <c r="M42" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
@@ -2093,22 +2404,27 @@
       <c r="I43" s="2">
         <v>2245</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="7">
+        <f>E43/I43</f>
+        <v>31.639643652561247</v>
+      </c>
+      <c r="K43" s="3">
         <f>F43/I43</f>
         <v>31.639643652561247</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L43" s="3">
-        <f>J43</f>
+      <c r="L43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M43" s="3">
+        <f>K43</f>
         <v>31.639643652561247</v>
       </c>
-      <c r="M43" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>62</v>
       </c>
@@ -2135,22 +2451,27 @@
       <c r="I44" s="3">
         <v>620</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="10">
+        <f>E44*H44*I44</f>
+        <v>19074.764999999999</v>
+      </c>
+      <c r="K44" s="3">
         <f>F44*H44*I44</f>
         <v>19074.764999999999</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L44" s="3">
-        <f>J44</f>
+      <c r="L44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" s="3">
+        <f>K44</f>
         <v>19074.764999999999</v>
       </c>
-      <c r="M44" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -2170,22 +2491,27 @@
       <c r="G45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="7">
         <f t="shared" si="0"/>
         <v>90113</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="3">
-        <f t="shared" ref="L45:L49" si="5">J45</f>
+      <c r="K45" s="3">
+        <f>F45</f>
         <v>90113</v>
       </c>
-      <c r="M45" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M45" s="3">
+        <f t="shared" ref="M45:M49" si="5">K45</f>
+        <v>90113</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>62</v>
       </c>
@@ -2208,22 +2534,27 @@
       <c r="I46" s="3">
         <v>1198.26</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="7">
+        <f>E46*I46/1000</f>
+        <v>10904.165999999999</v>
+      </c>
+      <c r="K46" s="3">
         <f>F46/1000*I46</f>
         <v>10904.165999999999</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L46" s="3">
+      <c r="L46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M46" s="3">
         <f t="shared" si="5"/>
         <v>10904.165999999999</v>
       </c>
-      <c r="M46" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>62</v>
       </c>
@@ -2250,30 +2581,35 @@
       <c r="I47" s="3">
         <v>30</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="10">
+        <f>E47*H47*I47</f>
+        <v>5823.9659999999994</v>
+      </c>
+      <c r="K47" s="3">
         <f>F47*H47*I47</f>
         <v>5823.9659999999994</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L47" s="3">
+      <c r="L47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M47" s="3">
         <f t="shared" si="5"/>
         <v>5823.9659999999994</v>
       </c>
-      <c r="M47" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O47" s="7"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E48" s="3">
         <v>503</v>
@@ -2288,22 +2624,27 @@
       <c r="I48" s="3">
         <v>1200</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="7">
+        <f>E48*I48/1000</f>
+        <v>603.6</v>
+      </c>
+      <c r="K48" s="3">
         <f>F48/1000*I48</f>
         <v>603.6</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L48" s="3">
+      <c r="L48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" s="3">
         <f t="shared" si="5"/>
         <v>603.6</v>
       </c>
-      <c r="M48" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
@@ -2323,22 +2664,27 @@
       <c r="G49" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="7">
         <f t="shared" si="0"/>
         <v>12078</v>
       </c>
-      <c r="K49" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L49" s="3">
+      <c r="K49" s="3">
+        <f>F49</f>
+        <v>12078</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49" s="3">
         <f t="shared" si="5"/>
         <v>12078</v>
       </c>
-      <c r="M49" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>62</v>
       </c>
@@ -2365,55 +2711,1944 @@
       <c r="I50" s="1">
         <v>675</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="10">
+        <f>E50*H50*I50</f>
+        <v>614326.78125</v>
+      </c>
+      <c r="K50" s="3">
         <f>F50*H50*I50</f>
         <v>614326.78125</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L50" s="3">
-        <f>J50</f>
+      <c r="L50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50" s="3">
+        <f>K50</f>
         <v>614326.78125</v>
       </c>
-      <c r="M50" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="concrete">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="concrete">
       <formula>NOT(ISERROR(SEARCH("concrete",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="concrete">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="concrete">
       <formula>NOT(ISERROR(SEARCH("concrete",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="mortar">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="mortar">
       <formula>NOT(ISERROR(SEARCH("mortar",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="mortar">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="mortar">
       <formula>NOT(ISERROR(SEARCH("mortar",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="mortar">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="mortar">
       <formula>NOT(ISERROR(SEARCH("mortar",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B1B820-FB86-4F2D-B26E-F834F8BFC4B2}">
+  <dimension ref="A1:N82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="13">
+        <f>B6/0.0929</f>
+        <v>89989.235737351992</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="11">
+        <v>8360</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="14">
+        <v>12</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="11">
+        <f>$B$6/$B$6</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>7415</v>
+      </c>
+      <c r="F11">
+        <f>E11*$B$8</f>
+        <v>7415</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11">
+        <f>F11</f>
+        <v>7415</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11">
+        <f>J11</f>
+        <v>7415</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>E12*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <v>450</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J49" si="0">F12</f>
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>285</v>
+      </c>
+      <c r="F13">
+        <f>E13*$B$8</f>
+        <v>285</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="16">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I13">
+        <v>70</v>
+      </c>
+      <c r="J13">
+        <f>F13*H13*I13</f>
+        <v>506.73</v>
+      </c>
+      <c r="K13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13">
+        <f>J13</f>
+        <v>506.73</v>
+      </c>
+      <c r="M13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>1548</v>
+      </c>
+      <c r="F14">
+        <f>E14*$B$8</f>
+        <v>1548</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <v>1198.26</v>
+      </c>
+      <c r="J14">
+        <f>F14/1000*I14</f>
+        <v>1854.9064800000001</v>
+      </c>
+      <c r="K14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L19" si="1">J14</f>
+        <v>1854.9064800000001</v>
+      </c>
+      <c r="M14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>144</v>
+      </c>
+      <c r="F15">
+        <f>E15*$B$8</f>
+        <v>144</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="16">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <f>F15*H15*I15</f>
+        <v>109.72799999999999</v>
+      </c>
+      <c r="K15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>109.72799999999999</v>
+      </c>
+      <c r="M15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16">
+        <v>5693</v>
+      </c>
+      <c r="F16">
+        <f>E16*$B$8</f>
+        <v>5693</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>5693</v>
+      </c>
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>5693</v>
+      </c>
+      <c r="M16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>5945</v>
+      </c>
+      <c r="F17">
+        <f>E17*$B$8</f>
+        <v>5945</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="16">
+        <f>0.0254*5/8</f>
+        <v>1.5875E-2</v>
+      </c>
+      <c r="I17" s="17">
+        <v>675</v>
+      </c>
+      <c r="J17">
+        <f>F17*H17*I17</f>
+        <v>63704.390625</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>63704.390625</v>
+      </c>
+      <c r="M17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18">
+        <v>3337</v>
+      </c>
+      <c r="F18">
+        <f>E18*$B$8</f>
+        <v>3337</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="16">
+        <f>0.0254*0.5</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="I18" s="17">
+        <v>675</v>
+      </c>
+      <c r="J18">
+        <f>F18*H18*I18</f>
+        <v>28606.432499999999</v>
+      </c>
+      <c r="K18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>28606.432499999999</v>
+      </c>
+      <c r="M18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>117</v>
+      </c>
+      <c r="F19">
+        <f>E19*$B$8</f>
+        <v>117</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19">
+        <v>1200</v>
+      </c>
+      <c r="J19">
+        <f>F19/1000*I19</f>
+        <v>140.4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>140.4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>E20*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20">
+        <v>450</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20">
+        <f>I20*J20</f>
+        <v>0</v>
+      </c>
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>110</v>
+      </c>
+      <c r="F21">
+        <f>E21*$B$8</f>
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="K21" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21">
+        <f>J21</f>
+        <v>110</v>
+      </c>
+      <c r="M21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22">
+        <v>400</v>
+      </c>
+      <c r="F22">
+        <f>E22*$B$8</f>
+        <v>400</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="K22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22">
+        <f>J22</f>
+        <v>400</v>
+      </c>
+      <c r="M22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>1878</v>
+      </c>
+      <c r="F23">
+        <f>E23*$B$8</f>
+        <v>1878</v>
+      </c>
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23">
+        <v>2245</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>1878</v>
+      </c>
+      <c r="K23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23">
+        <f>I23*J23</f>
+        <v>4216110</v>
+      </c>
+      <c r="M23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>4737</v>
+      </c>
+      <c r="F24">
+        <f>E24*$B$8</f>
+        <v>4737</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>4737</v>
+      </c>
+      <c r="K24" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24">
+        <f>J24</f>
+        <v>4737</v>
+      </c>
+      <c r="M24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25">
+        <v>661</v>
+      </c>
+      <c r="F25">
+        <f>E25*$B$8</f>
+        <v>661</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25">
+        <f>0.0254*3/8</f>
+        <v>9.5249999999999987E-3</v>
+      </c>
+      <c r="I25">
+        <v>620</v>
+      </c>
+      <c r="J25">
+        <f>F25*H25*I25</f>
+        <v>3903.5354999999995</v>
+      </c>
+      <c r="K25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25:L30" si="2">J25</f>
+        <v>3903.5354999999995</v>
+      </c>
+      <c r="M25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>4067</v>
+      </c>
+      <c r="F26">
+        <f>E26*$B$8</f>
+        <v>4067</v>
+      </c>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="16">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26">
+        <f>F26*H26*I26</f>
+        <v>3099.0540000000001</v>
+      </c>
+      <c r="K26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>3099.0540000000001</v>
+      </c>
+      <c r="M26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="18">
+        <v>170348</v>
+      </c>
+      <c r="F27">
+        <f>E27*$B$8</f>
+        <v>170348</v>
+      </c>
+      <c r="G27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>170348</v>
+      </c>
+      <c r="K27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>170348</v>
+      </c>
+      <c r="M27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28">
+        <v>875</v>
+      </c>
+      <c r="F28">
+        <f>E28*$B$8</f>
+        <v>875</v>
+      </c>
+      <c r="G28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>875</v>
+      </c>
+      <c r="K28" t="s">
+        <v>29</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>875</v>
+      </c>
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29">
+        <v>110</v>
+      </c>
+      <c r="F29">
+        <f>E29*$B$8</f>
+        <v>110</v>
+      </c>
+      <c r="G29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="K29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="M29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>351</v>
+      </c>
+      <c r="F30">
+        <f>E30*$B$8</f>
+        <v>351</v>
+      </c>
+      <c r="G30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30">
+        <f>0.0254/1000*60</f>
+        <v>1.5239999999999997E-3</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <f>F30*H30*I30</f>
+        <v>0.53492399999999996</v>
+      </c>
+      <c r="K30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>0.53492399999999996</v>
+      </c>
+      <c r="M30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31">
+        <v>149</v>
+      </c>
+      <c r="F31">
+        <f>E31*$B$8</f>
+        <v>149</v>
+      </c>
+      <c r="G31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31">
+        <v>2245</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="K31" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31">
+        <f>I31*J31</f>
+        <v>334505</v>
+      </c>
+      <c r="M31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="18">
+        <v>57884</v>
+      </c>
+      <c r="F32">
+        <f>E32*$B$8</f>
+        <v>57884</v>
+      </c>
+      <c r="G32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>57884</v>
+      </c>
+      <c r="K32" t="s">
+        <v>29</v>
+      </c>
+      <c r="L32">
+        <f>J32</f>
+        <v>57884</v>
+      </c>
+      <c r="M32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="18">
+        <v>39230</v>
+      </c>
+      <c r="F33">
+        <f>E33*$B$8</f>
+        <v>39230</v>
+      </c>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>39230</v>
+      </c>
+      <c r="K33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L34" si="3">J33</f>
+        <v>39230</v>
+      </c>
+      <c r="M33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34">
+        <v>60</v>
+      </c>
+      <c r="F34">
+        <f>E34*$B$8</f>
+        <v>60</v>
+      </c>
+      <c r="G34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="M34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35">
+        <v>162</v>
+      </c>
+      <c r="F35">
+        <f>E35*$B$8</f>
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35">
+        <v>2245</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="K35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35">
+        <f>I35*J35</f>
+        <v>363690</v>
+      </c>
+      <c r="M35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f>E36*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36">
+        <v>450</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36">
+        <f>I36*J36</f>
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="18">
+        <v>22089</v>
+      </c>
+      <c r="F37">
+        <f>E37*$B$8</f>
+        <v>22089</v>
+      </c>
+      <c r="G37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>22089</v>
+      </c>
+      <c r="K37" t="s">
+        <v>29</v>
+      </c>
+      <c r="L37">
+        <f>J37</f>
+        <v>22089</v>
+      </c>
+      <c r="M37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38">
+        <v>823</v>
+      </c>
+      <c r="F38">
+        <f>E38*$B$8</f>
+        <v>823</v>
+      </c>
+      <c r="G38" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>823</v>
+      </c>
+      <c r="K38" t="s">
+        <v>29</v>
+      </c>
+      <c r="L38">
+        <f t="shared" ref="L38:L39" si="4">J38</f>
+        <v>823</v>
+      </c>
+      <c r="M38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="18">
+        <v>31051</v>
+      </c>
+      <c r="F39">
+        <f>E39*$B$8</f>
+        <v>31051</v>
+      </c>
+      <c r="G39" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>31051</v>
+      </c>
+      <c r="K39" t="s">
+        <v>29</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="4"/>
+        <v>31051</v>
+      </c>
+      <c r="M39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f>E40*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40">
+        <v>450</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>31</v>
+      </c>
+      <c r="L40">
+        <f>I40*J40</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="18">
+        <v>30026</v>
+      </c>
+      <c r="F41">
+        <f>E41*$B$8</f>
+        <v>30026</v>
+      </c>
+      <c r="G41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>30026</v>
+      </c>
+      <c r="K41" t="s">
+        <v>29</v>
+      </c>
+      <c r="L41">
+        <f>J41</f>
+        <v>30026</v>
+      </c>
+      <c r="M41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42">
+        <v>438</v>
+      </c>
+      <c r="F42">
+        <f>E42*$B$8</f>
+        <v>438</v>
+      </c>
+      <c r="G42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42">
+        <v>2245</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>438</v>
+      </c>
+      <c r="K42" t="s">
+        <v>31</v>
+      </c>
+      <c r="L42">
+        <f>I42*J42</f>
+        <v>983310</v>
+      </c>
+      <c r="M42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="18">
+        <v>70908</v>
+      </c>
+      <c r="F43">
+        <f>E43*$B$8</f>
+        <v>70908</v>
+      </c>
+      <c r="G43" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43">
+        <v>2245</v>
+      </c>
+      <c r="J43">
+        <f>F43/I43</f>
+        <v>31.584855233853006</v>
+      </c>
+      <c r="K43" t="s">
+        <v>29</v>
+      </c>
+      <c r="L43">
+        <f>J43</f>
+        <v>31.584855233853006</v>
+      </c>
+      <c r="M43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44">
+        <v>3230</v>
+      </c>
+      <c r="F44">
+        <f>E44*$B$8</f>
+        <v>3230</v>
+      </c>
+      <c r="G44" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44">
+        <f>0.0254*3/8</f>
+        <v>9.5249999999999987E-3</v>
+      </c>
+      <c r="I44">
+        <v>620</v>
+      </c>
+      <c r="J44">
+        <f>F44*H44*I44</f>
+        <v>19074.764999999999</v>
+      </c>
+      <c r="K44" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44">
+        <f>J44</f>
+        <v>19074.764999999999</v>
+      </c>
+      <c r="M44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="18">
+        <v>89824</v>
+      </c>
+      <c r="F45">
+        <f>E45*$B$8</f>
+        <v>89824</v>
+      </c>
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>89824</v>
+      </c>
+      <c r="K45" t="s">
+        <v>29</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ref="L45:L50" si="5">J45</f>
+        <v>89824</v>
+      </c>
+      <c r="M45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46">
+        <v>5143</v>
+      </c>
+      <c r="F46">
+        <f>E46*$B$8</f>
+        <v>5143</v>
+      </c>
+      <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46">
+        <v>1198.26</v>
+      </c>
+      <c r="J46">
+        <f>F46/1000*I46</f>
+        <v>6162.6511799999998</v>
+      </c>
+      <c r="K46" t="s">
+        <v>29</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="5"/>
+        <v>6162.6511799999998</v>
+      </c>
+      <c r="M46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47">
+        <v>7644</v>
+      </c>
+      <c r="F47">
+        <f>E47*$B$8</f>
+        <v>7644</v>
+      </c>
+      <c r="G47" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47">
+        <f>0.0254</f>
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I47">
+        <v>30</v>
+      </c>
+      <c r="J47">
+        <f>F47*H47*I47</f>
+        <v>5824.7280000000001</v>
+      </c>
+      <c r="K47" t="s">
+        <v>29</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="5"/>
+        <v>5824.7280000000001</v>
+      </c>
+      <c r="M47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48">
+        <v>503</v>
+      </c>
+      <c r="F48">
+        <f>E48*$B$8</f>
+        <v>503</v>
+      </c>
+      <c r="G48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48">
+        <v>1200</v>
+      </c>
+      <c r="J48">
+        <f>F48/1000*I48</f>
+        <v>603.6</v>
+      </c>
+      <c r="K48" t="s">
+        <v>29</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="5"/>
+        <v>603.6</v>
+      </c>
+      <c r="M48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="18">
+        <v>125951</v>
+      </c>
+      <c r="F49">
+        <f>E49*$B$8</f>
+        <v>125951</v>
+      </c>
+      <c r="G49" t="s">
+        <v>29</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>125951</v>
+      </c>
+      <c r="K49" t="s">
+        <v>29</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="5"/>
+        <v>125951</v>
+      </c>
+      <c r="M49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" s="18">
+        <v>47097</v>
+      </c>
+      <c r="F50">
+        <f>E50*$B$8</f>
+        <v>47097</v>
+      </c>
+      <c r="G50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50">
+        <f>0.0254*5/8</f>
+        <v>1.5875E-2</v>
+      </c>
+      <c r="I50" s="17">
+        <v>675</v>
+      </c>
+      <c r="J50">
+        <f>F50*H50*I50</f>
+        <v>504673.79062500002</v>
+      </c>
+      <c r="K50" t="s">
+        <v>29</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="5"/>
+        <v>504673.79062500002</v>
+      </c>
+      <c r="M50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D58" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="15"/>
+      <c r="D59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="15"/>
+      <c r="D60" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="15"/>
+      <c r="D61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="15"/>
+      <c r="D62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="15"/>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" s="15"/>
+      <c r="D64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="15"/>
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="15"/>
+      <c r="D66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="15"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="15"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="15"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="15"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="15"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="15"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="15"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="15"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="15"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="15"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="15"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="15"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="15"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="15"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="15"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="15"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C8">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="concrete">
+      <formula>NOT(ISERROR(SEARCH("concrete",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="concrete">
+      <formula>NOT(ISERROR(SEARCH("concrete",D10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="concrete">
+      <formula>NOT(ISERROR(SEARCH("concrete",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",D20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="mortar">
+      <formula>NOT(ISERROR(SEARCH("mortar",D61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>